<commit_message>
glottosave fixes #41, #40
</commit_message>
<xml_diff>
--- a/glottosubdata.xlsx
+++ b/glottosubdata.xlsx
@@ -12,8 +12,9 @@
     <sheet name="structure" sheetId="3" r:id="rId3"/>
     <sheet name="metadata" sheetId="4" r:id="rId4"/>
     <sheet name="references" sheetId="5" r:id="rId5"/>
-    <sheet name="readme" sheetId="6" r:id="rId6"/>
-    <sheet name="lookup" sheetId="7" r:id="rId7"/>
+    <sheet name="remarks" sheetId="6" r:id="rId6"/>
+    <sheet name="readme" sheetId="7" r:id="rId7"/>
+    <sheet name="lookup" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -357,7 +358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,63 +396,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>yucu1253_a_0002</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>yucu1253_a_0003</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>yucu1253_a_0004</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>yucu1253_a_0005</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
           <t>yucu1253_b_0001</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>yucu1253_b_0002</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>yucu1253_b_0003</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>yucu1253_b_0004</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>yucu1253_b_0005</t>
         </is>
       </c>
     </row>
@@ -462,7 +407,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -500,63 +445,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>tani1257_a_0002</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>tani1257_a_0003</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>tani1257_a_0004</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>tani1257_a_0005</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
           <t>tani1257_b_0001</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>tani1257_b_0002</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>tani1257_b_0003</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>tani1257_b_0004</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>tani1257_b_0005</t>
         </is>
       </c>
     </row>
@@ -772,6 +661,55 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>glottocode</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>var001_remark</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>var002_remark</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>var003_remark</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>yucu1253</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tani1257</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -826,7 +764,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>version 0.0.7</t>
+          <t>version 0.0.71</t>
         </is>
       </c>
     </row>
@@ -835,7 +773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>

</xml_diff>